<commit_message>
simplified and re-benched TPCH q12
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/repos/sdql-rs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFF0941-25F7-D848-AF07-379025AAB243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283FB634-76B3-2446-891C-F020A2DF2879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35020" yWindow="500" windowWidth="33780" windowHeight="28300" xr2:uid="{350F099A-CA24-BB46-A12D-AAF0BFB2B0F0}"/>
   </bookViews>
@@ -562,12 +562,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -947,7 +945,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,233 +986,233 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>32</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>122</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <f>$B2/$C2</f>
         <v>0.26229508196721313</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>22</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <f>$C2/$E2</f>
         <v>5.5454545454545459</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>167</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <f>$G2/$C2</f>
         <v>1.3688524590163935</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <f t="shared" ref="D3:D23" si="0">$B3/$C3</f>
         <v>1.6</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <f t="shared" ref="F3:F23" si="1">$C3/$E3</f>
         <v>2.5</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>12</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <f t="shared" ref="H3:H23" si="2">$G3/$C3</f>
         <v>2.4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>38</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>64</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <f t="shared" si="0"/>
         <v>0.59375</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>12</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <f t="shared" si="1"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>54</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <f t="shared" si="2"/>
         <v>0.84375</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>24</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>39</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
         <v>0.61538461538461542</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>8</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <f t="shared" si="1"/>
         <v>4.875</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>63</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <f t="shared" si="2"/>
         <v>1.6153846153846154</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>44</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>52</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <f t="shared" si="0"/>
         <v>0.84615384615384615</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>11</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <f t="shared" si="1"/>
         <v>4.7272727272727275</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>61</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <f t="shared" si="2"/>
         <v>1.1730769230769231</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>24</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>32</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7">
         <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <v>34</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7">
         <f t="shared" si="2"/>
         <v>1.0625</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>47</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>110</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>0.42727272727272725</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>36</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8">
         <f t="shared" si="1"/>
         <v>3.0555555555555554</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>156</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8">
         <f t="shared" si="2"/>
         <v>1.4181818181818182</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>69</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>161</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9">
         <v>93</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9">
         <f t="shared" si="1"/>
         <v>1.7311827956989247</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>37</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="3">
         <f t="shared" si="2"/>
         <v>0.22981366459627328</v>
       </c>
@@ -1224,375 +1222,374 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>104</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>201</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>0.51741293532338306</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10">
         <v>150</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10">
         <f t="shared" si="1"/>
         <v>1.34</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>141</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10">
         <f t="shared" si="2"/>
         <v>0.70149253731343286</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>272</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>103</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>2.6407766990291264</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11">
         <v>81</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11">
         <f t="shared" si="1"/>
         <v>1.271604938271605</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11">
         <v>113</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11">
         <f t="shared" si="2"/>
         <v>1.0970873786407767</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>10</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>11</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12">
         <v>10</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12">
         <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12">
         <v>5</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12">
         <f t="shared" si="2"/>
         <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>76</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>69</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>1.1014492753623188</v>
       </c>
-      <c r="E13" s="2">
-        <v>76</v>
-      </c>
-      <c r="F13" s="2">
-        <f t="shared" si="1"/>
-        <v>0.90789473684210531</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="E13">
+        <v>58</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>1.1896551724137931</v>
+      </c>
+      <c r="G13">
         <v>113</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13">
         <f t="shared" si="2"/>
         <v>1.6376811594202898</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>102</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>145</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>0.70344827586206893</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14">
         <v>58</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14">
         <v>119</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14">
         <f t="shared" si="2"/>
         <v>0.82068965517241377</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
         <v>8</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>44</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="1">
         <f t="shared" si="0"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15">
         <v>6</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15">
         <f t="shared" si="1"/>
         <v>7.333333333333333</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15">
         <v>31</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15">
         <f t="shared" si="2"/>
         <v>0.70454545454545459</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <v>10</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>47</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="1">
         <f t="shared" si="0"/>
         <v>0.21276595744680851</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16">
         <v>15</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16">
         <f t="shared" si="1"/>
         <v>3.1333333333333333</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16">
         <v>50</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16">
         <f t="shared" si="2"/>
         <v>1.0638297872340425</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17">
         <v>26</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>14</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>1.8571428571428572</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17">
         <v>44</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17">
         <f t="shared" si="1"/>
         <v>0.31818181818181818</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17">
         <v>18</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17">
         <f t="shared" si="2"/>
         <v>1.2857142857142858</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <v>131</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>119</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>1.1008403361344539</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18">
         <v>19</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18">
         <f t="shared" si="1"/>
         <v>6.2631578947368425</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18">
         <v>43</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18">
         <f t="shared" si="2"/>
         <v>0.36134453781512604</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
         <v>118</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>117</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>1.0085470085470085</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19">
         <v>114</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19">
         <f t="shared" si="1"/>
         <v>1.0263157894736843</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19">
         <v>384</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19">
         <f t="shared" si="2"/>
         <v>3.2820512820512819</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <v>202</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>74</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>2.7297297297297298</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20">
         <v>153</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20">
         <f t="shared" si="1"/>
         <v>0.48366013071895425</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20">
         <v>149</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20">
         <f t="shared" si="2"/>
         <v>2.0135135135135136</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
         <v>18</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>55</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>0.32727272727272727</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21">
         <v>10</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21">
         <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21">
         <v>39</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21">
         <f t="shared" si="2"/>
         <v>0.70909090909090911</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22">
         <v>274</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>671</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>0.40834575260804767</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2">
+      <c r="G22">
         <v>148</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="3">
         <f t="shared" si="2"/>
         <v>0.22056631892697467</v>
       </c>
@@ -1602,49 +1599,44 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23">
         <v>3</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23">
         <v>2</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23">
         <v>26</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3">
+      <c r="D24" s="1">
         <f>AVERAGE(D2:D23)</f>
         <v>0.94191219748715715</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3">
+      <c r="F24" s="1">
         <f>AVERAGE(F2:F23)</f>
-        <v>3.1592990920098467</v>
-      </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="3">
+        <v>3.1727162556084987</v>
+      </c>
+      <c r="H24" s="1">
         <f>AVERAGE(H2:H23)</f>
         <v>1.70289598882909</v>
       </c>

</xml_diff>

<commit_message>
bool instead of int
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/repos/sdql-rs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52D97F4-F7F7-2541-A964-5206551D2A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0119C2-3649-0E40-9E81-66AAED893F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35020" yWindow="500" windowWidth="33780" windowHeight="28300" xr2:uid="{350F099A-CA24-BB46-A12D-AAF0BFB2B0F0}"/>
+    <workbookView xWindow="1240" yWindow="520" windowWidth="33760" windowHeight="28300" xr2:uid="{350F099A-CA24-BB46-A12D-AAF0BFB2B0F0}"/>
   </bookViews>
   <sheets>
     <sheet name="benchmarks" sheetId="1" r:id="rId1"/>
@@ -945,7 +945,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1080,25 +1080,25 @@
         <v>24</v>
       </c>
       <c r="C5">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>0.61538461538461542</v>
+        <v>0.64864864864864868</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>4.875</v>
+        <v>6.166666666666667</v>
       </c>
       <c r="G5">
         <v>63</v>
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>1.6153846153846154</v>
+        <v>1.7027027027027026</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1577,11 +1577,11 @@
         <v>274</v>
       </c>
       <c r="C22">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>0.40834575260804767</v>
+        <v>0.40652818991097922</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
@@ -1591,11 +1591,11 @@
       </c>
       <c r="H22" s="3">
         <f t="shared" si="2"/>
-        <v>0.22056631892697467</v>
+        <v>0.21958456973293769</v>
       </c>
       <c r="I22" s="1">
         <f>1/H22</f>
-        <v>4.5337837837837833</v>
+        <v>4.5540540540540544</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1613,11 +1613,11 @@
         <v>1.5</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G23">
         <v>26</v>
@@ -1630,15 +1630,15 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D24" s="1">
         <f>AVERAGE(D2:D23)</f>
-        <v>0.94498500772576077</v>
+        <v>0.94641439275153172</v>
       </c>
       <c r="F24" s="1">
         <f>AVERAGE(F2:F23)</f>
-        <v>3.152748624933063</v>
+        <v>3.1983835455679848</v>
       </c>
       <c r="H24" s="1">
         <f>AVERAGE(H2:H23)</f>
-        <v>1.7189322172618029</v>
+        <v>1.7228565962674416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Q21 smallvec (re-benched after updating nightly)
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/repos/sdql-rs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0119C2-3649-0E40-9E81-66AAED893F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E22F87-54CB-EA48-BEB4-E686B915FB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="520" windowWidth="33760" windowHeight="28300" xr2:uid="{350F099A-CA24-BB46-A12D-AAF0BFB2B0F0}"/>
+    <workbookView xWindow="1260" yWindow="500" windowWidth="33760" windowHeight="28300" xr2:uid="{350F099A-CA24-BB46-A12D-AAF0BFB2B0F0}"/>
   </bookViews>
   <sheets>
     <sheet name="benchmarks" sheetId="1" r:id="rId1"/>
@@ -945,7 +945,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1577,11 +1577,11 @@
         <v>274</v>
       </c>
       <c r="C22">
-        <v>674</v>
+        <v>587</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>0.40652818991097922</v>
+        <v>0.46678023850085176</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
@@ -1591,11 +1591,11 @@
       </c>
       <c r="H22" s="3">
         <f t="shared" si="2"/>
-        <v>0.21958456973293769</v>
+        <v>0.25212947189097101</v>
       </c>
       <c r="I22" s="1">
         <f>1/H22</f>
-        <v>4.5540540540540544</v>
+        <v>3.9662162162162167</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1630,7 +1630,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D24" s="1">
         <f>AVERAGE(D2:D23)</f>
-        <v>0.94641439275153172</v>
+        <v>0.94915312223288961</v>
       </c>
       <c r="F24" s="1">
         <f>AVERAGE(F2:F23)</f>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="H24" s="1">
         <f>AVERAGE(H2:H23)</f>
-        <v>1.7228565962674416</v>
+        <v>1.7243359100018978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated averages to use geomean + added DuckDB parallel results
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/repos/sdql-rs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAEBB73-A226-F943-977E-BC9BA771F18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767B49AF-8EC8-8042-8EF3-532D449F68BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="500" windowWidth="33760" windowHeight="28300" xr2:uid="{350F099A-CA24-BB46-A12D-AAF0BFB2B0F0}"/>
+    <workbookView xWindow="35020" yWindow="520" windowWidth="33780" windowHeight="28300" xr2:uid="{350F099A-CA24-BB46-A12D-AAF0BFB2B0F0}"/>
   </bookViews>
   <sheets>
     <sheet name="benchmarks" sheetId="1" r:id="rId1"/>
@@ -33,15 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Query</t>
   </si>
   <si>
     <t>SDQL (mean ms)</t>
-  </si>
-  <si>
-    <t>DuckDB (mean ms)</t>
   </si>
   <si>
     <t>sdql-rs</t>
@@ -60,6 +57,21 @@
   </si>
   <si>
     <t>sdql-rs vs DuckDB</t>
+  </si>
+  <si>
+    <t>DuckDB</t>
+  </si>
+  <si>
+    <t>DuckDB (parallel)</t>
+  </si>
+  <si>
+    <t>sdql-rs vs DuckDB (par)</t>
+  </si>
+  <si>
+    <t>DuckDB (par vs seq)</t>
+  </si>
+  <si>
+    <t>max ^</t>
   </si>
 </sst>
 </file>
@@ -942,24 +954,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D7B490-4574-3448-A408-3C33C96126ED}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -967,25 +983,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1010,11 +1035,22 @@
         <v>167</v>
       </c>
       <c r="H2">
+        <v>22</v>
+      </c>
+      <c r="I2">
+        <f>$G2/$H2</f>
+        <v>7.5909090909090908</v>
+      </c>
+      <c r="J2">
         <f>$G2/$C2</f>
         <v>2.141025641025641</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <f>$H2/E2</f>
+        <v>1.1578947368421053</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1039,11 +1075,22 @@
         <v>12</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H23" si="2">$G3/$C3</f>
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I23" si="2">$G3/$H3</f>
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J23" si="3">$G3/$C3</f>
         <v>2.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <f>$H3/E3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1068,11 +1115,22 @@
         <v>54</v>
       </c>
       <c r="H4">
+        <v>14</v>
+      </c>
+      <c r="I4">
         <f t="shared" si="2"/>
+        <v>3.8571428571428572</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
         <v>0.84375</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <f>$H4/E4</f>
+        <v>1.0769230769230769</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1097,11 +1155,22 @@
         <v>63</v>
       </c>
       <c r="H5">
+        <v>15</v>
+      </c>
+      <c r="I5">
         <f t="shared" si="2"/>
+        <v>4.2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
         <v>1.7027027027027026</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <f>$H5/E5</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1126,11 +1195,22 @@
         <v>61</v>
       </c>
       <c r="H6">
+        <v>14</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="2"/>
+        <v>4.3571428571428568</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
         <v>1.1730769230769231</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <f>$H6/E6</f>
+        <v>1.2727272727272727</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1155,11 +1235,22 @@
         <v>34</v>
       </c>
       <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="2"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
         <v>1.0625</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <f>$H7/E7</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1184,11 +1275,22 @@
         <v>156</v>
       </c>
       <c r="H8">
+        <v>38</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="2"/>
+        <v>4.1052631578947372</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
         <v>1.4181818181818182</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <f>$H8/E8</f>
+        <v>1.0857142857142856</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1212,16 +1314,23 @@
       <c r="G9">
         <v>37</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9">
+        <v>13</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="2"/>
+        <v>2.8461538461538463</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="3"/>
         <v>0.22699386503067484</v>
       </c>
-      <c r="I9" s="1">
-        <f>1/H9</f>
-        <v>4.4054054054054053</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <f>$H9/E9</f>
+        <v>0.13978494623655913</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1246,11 +1355,22 @@
         <v>141</v>
       </c>
       <c r="H10">
+        <v>32</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="2"/>
+        <v>4.40625</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
         <v>0.70149253731343286</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <f>$H10/E10</f>
+        <v>0.21768707482993196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1275,11 +1395,22 @@
         <v>113</v>
       </c>
       <c r="H11">
+        <v>36</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="2"/>
+        <v>3.1388888888888888</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
         <v>1.0865384615384615</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <f>$H11/E11</f>
+        <v>0.43373493975903615</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1304,11 +1435,22 @@
         <v>5</v>
       </c>
       <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="2"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
         <v>0.45454545454545453</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <f>$H12/E12</f>
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1333,11 +1475,22 @@
         <v>113</v>
       </c>
       <c r="H13">
+        <v>18</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="2"/>
+        <v>6.2777777777777777</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
         <v>1.6142857142857143</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <f>$H13/E13</f>
+        <v>0.31034482758620691</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1362,11 +1515,22 @@
         <v>119</v>
       </c>
       <c r="H14">
+        <v>29</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="2"/>
+        <v>4.1034482758620694</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
         <v>0.82638888888888884</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <f>$H14/E14</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1391,11 +1555,22 @@
         <v>31</v>
       </c>
       <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="2"/>
+        <v>3.1</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
         <v>0.70454545454545459</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <f>$H15/E15</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1420,11 +1595,22 @@
         <v>50</v>
       </c>
       <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
         <v>1.0869565217391304</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <f>$H16/E16</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1449,11 +1635,22 @@
         <v>18</v>
       </c>
       <c r="H17">
+        <v>9</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
         <v>1.2857142857142858</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <f>$H17/E17</f>
+        <v>0.20454545454545456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1478,11 +1675,22 @@
         <v>43</v>
       </c>
       <c r="H18">
+        <v>11</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="2"/>
+        <v>3.9090909090909092</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
         <v>0.37719298245614036</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <f>$H18/E18</f>
+        <v>0.57894736842105265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1507,11 +1715,22 @@
         <v>384</v>
       </c>
       <c r="H19">
+        <v>63</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="2"/>
+        <v>6.0952380952380949</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
         <v>3.2542372881355934</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <f>$H19/E19</f>
+        <v>0.57798165137614677</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1536,11 +1755,22 @@
         <v>149</v>
       </c>
       <c r="H20">
+        <v>28</v>
+      </c>
+      <c r="I20">
         <f t="shared" si="2"/>
+        <v>5.3214285714285712</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
         <v>2.0694444444444446</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <f>$H20/E20</f>
+        <v>0.18300653594771241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1565,11 +1795,22 @@
         <v>39</v>
       </c>
       <c r="H21">
+        <v>9</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="2"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
         <v>0.72222222222222221</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <f>$H21/E21</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1584,21 +1825,27 @@
         <v>0.45214521452145212</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G22">
         <v>148</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22">
+        <v>38</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="2"/>
+        <v>3.8947368421052633</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" si="3"/>
         <v>0.24422442244224424</v>
       </c>
-      <c r="I22" s="1">
-        <f>1/H22</f>
-        <v>4.0945945945945947</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1623,22 +1870,66 @@
         <v>26</v>
       </c>
       <c r="H23">
+        <v>13</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <f>$H23/E23</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D24" s="1">
-        <f>AVERAGE(D2:D23)</f>
-        <v>0.95599272037956773</v>
+        <f>ROUND(GEOMEAN(D2:D23),2)</f>
+        <v>0.74</v>
       </c>
       <c r="F24" s="1">
-        <f>AVERAGE(F2:F23)</f>
-        <v>3.1194052925400961</v>
-      </c>
-      <c r="H24" s="1">
-        <f>AVERAGE(H2:H23)</f>
-        <v>1.7452736194676921</v>
+        <f>ROUND(GEOMEAN(F2:F23),2)</f>
+        <v>2.27</v>
+      </c>
+      <c r="I24" s="1">
+        <f>ROUND(GEOMEAN(I2:I23),2)</f>
+        <v>3.8</v>
+      </c>
+      <c r="J24" s="1">
+        <f>ROUND(GEOMEAN(J2:J23),2)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K24" s="1">
+        <f>ROUND(GEOMEAN(K2:K23),2)</f>
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D25" s="2">
+        <f>ROUND(MAX(D2:D23),2)</f>
+        <v>2.81</v>
+      </c>
+      <c r="F25">
+        <f>ROUND(MAX(F2:F23),2)</f>
+        <v>7.33</v>
+      </c>
+      <c r="I25">
+        <f>ROUND(MAX(I2:I23),2)</f>
+        <v>7.59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>